<commit_message>
cd: update the forms.
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/DRC/cd_sch_sth_baseline_2_child_202202.xlsx
+++ b/SCH-STH/Impact assessments/DRC/cd_sch_sth_baseline_2_child_202202.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -282,10 +282,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>2. SCH/STH - Fiche  individuelle  d’inscription V2</t>
-  </si>
-  <si>
-    <t>cd_sch_sth_baseline_2_child_202202_v2</t>
+    <t>2. SCH/STH - Fiche  individuelle  d’inscription V2.1</t>
+  </si>
+  <si>
+    <t>cd_sch_sth_baseline_2_child_202202_v2_1</t>
   </si>
   <si>
     <t>French</t>
@@ -326,6 +326,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -334,16 +342,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -355,6 +386,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -363,64 +462,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -431,51 +476,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -492,19 +492,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,163 +672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,6 +712,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -727,11 +760,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -739,7 +778,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -759,201 +809,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1354,7 +1354,7 @@
   <sheetPr/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2082,8 +2082,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>